<commit_message>
Added EDA3 in entirety
</commit_message>
<xml_diff>
--- a/Hospitalizations.xlsx
+++ b/Hospitalizations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rose Thorne\Desktop\ASC\Fall24\DirectedResearch\EDA_22Sept24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{BD9D9399-737A-4F18-B51E-94D8818E7D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B028B2-D536-4509-AFE3-D6226574F176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{413F0014-6665-4488-8B5A-7D188F1DB693}"/>
+    <workbookView xWindow="30690" yWindow="360" windowWidth="23565" windowHeight="15060" xr2:uid="{413F0014-6665-4488-8B5A-7D188F1DB693}"/>
   </bookViews>
   <sheets>
     <sheet name="data_225644" sheetId="1" r:id="rId1"/>
@@ -1020,9 +1020,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0757512F-8CEF-4F10-9E5C-AA37995B0CE9}">
   <dimension ref="A1:G1311"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>